<commit_message>
updating files and scripts
</commit_message>
<xml_diff>
--- a/var_info/indv_panel_var_info/ADDHEALTH_VariableInfo.xlsx
+++ b/var_info/indv_panel_var_info/ADDHEALTH_VariableInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/CDS-Data/08_Projects/TSRP/var_info/indv_panel_var_info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/CDS-Data/08_Projects/temprisk/var_info/indv_panel_var_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A895E6B7-497A-0A41-907E-F008B2EBFFC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBFC269-C40B-6D4E-B6D2-495B722D69C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="20660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51600" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Measures" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,14 @@
     <sheet name="PanelInfo" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Measures!$A$1:$O$185</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Measures!$A$1:$P$185</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="344">
   <si>
     <t>ord</t>
   </si>
@@ -1057,6 +1057,9 @@
   </si>
   <si>
     <t>CIGS_MO_DIS31A</t>
+  </si>
+  <si>
+    <t>item_num</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1133,7 +1136,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1448,11 +1450,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O185"/>
+  <dimension ref="A1:P185"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N186" sqref="N186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1462,7 +1464,7 @@
     <col min="5" max="5" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>148</v>
       </c>
@@ -1506,10 +1508,13 @@
         <v>155</v>
       </c>
       <c r="O1" t="s">
+        <v>343</v>
+      </c>
+      <c r="P1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -1543,8 +1548,11 @@
       <c r="K2">
         <v>365</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="O2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -1578,8 +1586,11 @@
       <c r="K3">
         <v>365</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -1613,8 +1624,11 @@
       <c r="K4">
         <v>365</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="O4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -1648,11 +1662,14 @@
       <c r="K5">
         <v>365</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -1686,11 +1703,14 @@
       <c r="K6">
         <v>365</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -1724,8 +1744,11 @@
       <c r="K7">
         <v>365</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="O7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -1759,8 +1782,11 @@
       <c r="K8">
         <v>365</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -1794,8 +1820,11 @@
       <c r="K9">
         <v>365</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>93</v>
       </c>
@@ -1829,8 +1858,11 @@
       <c r="K10">
         <v>365</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>93</v>
       </c>
@@ -1864,8 +1896,11 @@
       <c r="K11">
         <v>365</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>93</v>
       </c>
@@ -1899,8 +1934,11 @@
       <c r="K12">
         <v>365</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -1934,8 +1972,11 @@
       <c r="K13">
         <v>365</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -1969,8 +2010,11 @@
       <c r="K14">
         <v>365</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="O14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -2004,8 +2048,11 @@
       <c r="K15">
         <v>365</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="O15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -2039,8 +2086,11 @@
       <c r="K16">
         <v>365</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="O16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>93</v>
       </c>
@@ -2074,8 +2124,11 @@
       <c r="K17">
         <v>365</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -2109,8 +2162,11 @@
       <c r="K18">
         <v>365</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="O18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>93</v>
       </c>
@@ -2144,8 +2200,11 @@
       <c r="K19">
         <v>365</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="O19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -2179,8 +2238,11 @@
       <c r="K20">
         <v>365</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="O20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -2214,8 +2276,11 @@
       <c r="K21">
         <v>365</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="O21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -2249,8 +2314,11 @@
       <c r="K22">
         <v>365</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="O22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -2284,8 +2352,11 @@
       <c r="K23">
         <v>365</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="O23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -2319,8 +2390,11 @@
       <c r="K24">
         <v>365</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="O24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>93</v>
       </c>
@@ -2354,8 +2428,11 @@
       <c r="K25">
         <v>365</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="O25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -2389,8 +2466,11 @@
       <c r="K26">
         <v>365</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="O26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>93</v>
       </c>
@@ -2424,8 +2504,11 @@
       <c r="K27">
         <v>365</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" ht="19">
+      <c r="O27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="19">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -2460,8 +2543,11 @@
         <v>365</v>
       </c>
       <c r="N28" s="3"/>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="O28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>93</v>
       </c>
@@ -2495,8 +2581,11 @@
       <c r="K29">
         <v>365</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="O29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" t="s">
         <v>93</v>
       </c>
@@ -2530,8 +2619,11 @@
       <c r="K30">
         <v>365</v>
       </c>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="O30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" t="s">
         <v>93</v>
       </c>
@@ -2565,11 +2657,14 @@
       <c r="K31">
         <v>365</v>
       </c>
-      <c r="O31" t="s">
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:16">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -2603,11 +2698,14 @@
       <c r="K32">
         <v>365</v>
       </c>
-      <c r="O32" t="s">
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>93</v>
       </c>
@@ -2641,8 +2739,11 @@
       <c r="K33">
         <v>365</v>
       </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="O33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -2676,8 +2777,11 @@
       <c r="K34">
         <v>365</v>
       </c>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="O34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -2711,8 +2815,11 @@
       <c r="K35">
         <v>365</v>
       </c>
-    </row>
-    <row r="36" spans="1:14">
+      <c r="O35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -2746,8 +2853,11 @@
       <c r="N36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="O36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>93</v>
       </c>
@@ -2781,8 +2891,11 @@
       <c r="N37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="O37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>93</v>
       </c>
@@ -2816,8 +2929,11 @@
       <c r="N38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="O38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -2851,8 +2967,11 @@
       <c r="N39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="O39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>93</v>
       </c>
@@ -2886,8 +3005,11 @@
       <c r="N40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:14">
+      <c r="O40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>93</v>
       </c>
@@ -2918,8 +3040,11 @@
       <c r="K41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:14">
+      <c r="O41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>93</v>
       </c>
@@ -2950,8 +3075,11 @@
       <c r="K42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:14">
+      <c r="O42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>93</v>
       </c>
@@ -2982,8 +3110,11 @@
       <c r="K43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:14">
+      <c r="O43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
         <v>93</v>
       </c>
@@ -3014,8 +3145,11 @@
       <c r="K44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:14">
+      <c r="O44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
         <v>93</v>
       </c>
@@ -3046,8 +3180,11 @@
       <c r="K45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:14">
+      <c r="O45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -3078,8 +3215,11 @@
       <c r="K46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:14">
+      <c r="O46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>93</v>
       </c>
@@ -3113,8 +3253,11 @@
       <c r="K47">
         <v>30</v>
       </c>
-    </row>
-    <row r="48" spans="1:14">
+      <c r="O47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -3148,8 +3291,11 @@
       <c r="K48">
         <v>30</v>
       </c>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="O48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="A49" t="s">
         <v>93</v>
       </c>
@@ -3183,11 +3329,14 @@
       <c r="K49">
         <v>365</v>
       </c>
-      <c r="O49" t="s">
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:16">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -3221,11 +3370,14 @@
       <c r="K50">
         <v>365</v>
       </c>
-      <c r="O50" t="s">
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:16">
       <c r="A51" t="s">
         <v>93</v>
       </c>
@@ -3259,8 +3411,11 @@
       <c r="K51">
         <v>365</v>
       </c>
-    </row>
-    <row r="52" spans="1:15">
+      <c r="O51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52" t="s">
         <v>93</v>
       </c>
@@ -3294,8 +3449,11 @@
       <c r="K52">
         <v>365</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" ht="19" customHeight="1">
+      <c r="O52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="19" customHeight="1">
       <c r="A53" t="s">
         <v>93</v>
       </c>
@@ -3329,8 +3487,11 @@
       <c r="K53">
         <v>365</v>
       </c>
-    </row>
-    <row r="54" spans="1:15">
+      <c r="O53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54" t="s">
         <v>93</v>
       </c>
@@ -3364,8 +3525,11 @@
       <c r="N54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:15">
+      <c r="O54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55" t="s">
         <v>93</v>
       </c>
@@ -3399,8 +3563,11 @@
       <c r="K55">
         <v>30</v>
       </c>
-    </row>
-    <row r="56" spans="1:15">
+      <c r="O55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
       <c r="A56" t="s">
         <v>93</v>
       </c>
@@ -3434,8 +3601,11 @@
       <c r="K56">
         <v>30</v>
       </c>
-    </row>
-    <row r="57" spans="1:15">
+      <c r="O56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
       <c r="A57" t="s">
         <v>93</v>
       </c>
@@ -3469,8 +3639,11 @@
       <c r="N57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:15">
+      <c r="O57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -3504,8 +3677,11 @@
       <c r="N58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:15">
+      <c r="O58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
       <c r="A59" t="s">
         <v>93</v>
       </c>
@@ -3539,8 +3715,11 @@
       <c r="N59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:15">
+      <c r="O59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
       <c r="A60" t="s">
         <v>93</v>
       </c>
@@ -3574,8 +3753,11 @@
       <c r="N60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:15">
+      <c r="O60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
       <c r="A61" t="s">
         <v>93</v>
       </c>
@@ -3609,8 +3791,11 @@
       <c r="N61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:15">
+      <c r="O61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
       <c r="A62" t="s">
         <v>93</v>
       </c>
@@ -3644,8 +3829,11 @@
       <c r="N62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:15">
+      <c r="O62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
       <c r="A63" t="s">
         <v>93</v>
       </c>
@@ -3679,8 +3867,11 @@
       <c r="N63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:15">
+      <c r="O63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
       <c r="A64" t="s">
         <v>93</v>
       </c>
@@ -3714,8 +3905,11 @@
       <c r="N64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:14">
+      <c r="O64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" t="s">
         <v>93</v>
       </c>
@@ -3746,8 +3940,11 @@
       <c r="K65">
         <v>30</v>
       </c>
-    </row>
-    <row r="66" spans="1:14">
+      <c r="O65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" t="s">
         <v>93</v>
       </c>
@@ -3778,8 +3975,11 @@
       <c r="K66">
         <v>30</v>
       </c>
-    </row>
-    <row r="67" spans="1:14">
+      <c r="O66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67" t="s">
         <v>93</v>
       </c>
@@ -3810,8 +4010,11 @@
       <c r="K67">
         <v>30</v>
       </c>
-    </row>
-    <row r="68" spans="1:14">
+      <c r="O67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68" t="s">
         <v>93</v>
       </c>
@@ -3845,8 +4048,11 @@
       <c r="K68">
         <v>30</v>
       </c>
-    </row>
-    <row r="69" spans="1:14">
+      <c r="O68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69" t="s">
         <v>93</v>
       </c>
@@ -3880,8 +4086,11 @@
       <c r="K69">
         <v>30</v>
       </c>
-    </row>
-    <row r="70" spans="1:14">
+      <c r="O69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70" t="s">
         <v>93</v>
       </c>
@@ -3915,8 +4124,11 @@
       <c r="N70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:14">
+      <c r="O70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
       <c r="A71" t="s">
         <v>93</v>
       </c>
@@ -3950,8 +4162,11 @@
       <c r="N71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:14">
+      <c r="O71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
       <c r="A72" t="s">
         <v>93</v>
       </c>
@@ -3985,8 +4200,11 @@
       <c r="N72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:14">
+      <c r="O72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
       <c r="A73" t="s">
         <v>93</v>
       </c>
@@ -4020,8 +4238,11 @@
       <c r="N73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:14">
+      <c r="O73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
       <c r="A74" t="s">
         <v>93</v>
       </c>
@@ -4052,8 +4273,11 @@
       <c r="K74">
         <v>30</v>
       </c>
-    </row>
-    <row r="75" spans="1:14">
+      <c r="O74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75" t="s">
         <v>93</v>
       </c>
@@ -4084,8 +4308,11 @@
       <c r="K75">
         <v>30</v>
       </c>
-    </row>
-    <row r="76" spans="1:14">
+      <c r="O75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76" t="s">
         <v>93</v>
       </c>
@@ -4116,8 +4343,11 @@
       <c r="K76">
         <v>30</v>
       </c>
-    </row>
-    <row r="77" spans="1:14">
+      <c r="O76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
       <c r="A77" t="s">
         <v>93</v>
       </c>
@@ -4151,8 +4381,11 @@
       <c r="N77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:14">
+      <c r="O77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
       <c r="A78" t="s">
         <v>93</v>
       </c>
@@ -4186,8 +4419,11 @@
       <c r="N78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:14">
+      <c r="O78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79" t="s">
         <v>93</v>
       </c>
@@ -4221,8 +4457,11 @@
       <c r="N79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:14">
+      <c r="O79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
       <c r="A80" t="s">
         <v>93</v>
       </c>
@@ -4256,8 +4495,11 @@
       <c r="N80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:14">
+      <c r="O80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
       <c r="A81" t="s">
         <v>93</v>
       </c>
@@ -4291,8 +4533,11 @@
       <c r="N81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:14">
+      <c r="O81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
       <c r="A82" t="s">
         <v>93</v>
       </c>
@@ -4326,8 +4571,11 @@
       <c r="N82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:14">
+      <c r="O82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
       <c r="A83" t="s">
         <v>93</v>
       </c>
@@ -4361,8 +4609,11 @@
       <c r="N83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:14">
+      <c r="O83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
       <c r="A84" t="s">
         <v>93</v>
       </c>
@@ -4393,8 +4644,11 @@
       <c r="K84">
         <v>30</v>
       </c>
-    </row>
-    <row r="85" spans="1:14">
+      <c r="O84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -4425,8 +4679,11 @@
       <c r="K85">
         <v>30</v>
       </c>
-    </row>
-    <row r="86" spans="1:14">
+      <c r="O85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -4457,8 +4714,11 @@
       <c r="K86">
         <v>30</v>
       </c>
-    </row>
-    <row r="87" spans="1:14">
+      <c r="O86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -4489,8 +4749,11 @@
       <c r="K87">
         <v>30</v>
       </c>
-    </row>
-    <row r="88" spans="1:14">
+      <c r="O87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
       <c r="A88" t="s">
         <v>93</v>
       </c>
@@ -4521,8 +4784,11 @@
       <c r="K88">
         <v>30</v>
       </c>
-    </row>
-    <row r="89" spans="1:14">
+      <c r="O88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
       <c r="A89" t="s">
         <v>93</v>
       </c>
@@ -4556,8 +4822,11 @@
       <c r="N89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:14">
+      <c r="O89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -4591,8 +4860,11 @@
       <c r="N90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:14">
+      <c r="O90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15">
       <c r="A91" t="s">
         <v>93</v>
       </c>
@@ -4623,8 +4895,11 @@
       <c r="K91">
         <v>30</v>
       </c>
-    </row>
-    <row r="92" spans="1:14">
+      <c r="O91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15">
       <c r="A92" t="s">
         <v>93</v>
       </c>
@@ -4655,8 +4930,11 @@
       <c r="K92">
         <v>30</v>
       </c>
-    </row>
-    <row r="93" spans="1:14">
+      <c r="O92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -4690,8 +4968,11 @@
       <c r="K93">
         <v>365</v>
       </c>
-    </row>
-    <row r="94" spans="1:14">
+      <c r="O93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -4725,8 +5006,11 @@
       <c r="K94">
         <v>365</v>
       </c>
-    </row>
-    <row r="95" spans="1:14">
+      <c r="O94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -4760,8 +5044,11 @@
       <c r="K95">
         <v>365</v>
       </c>
-    </row>
-    <row r="96" spans="1:14">
+      <c r="O95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15">
       <c r="A96" t="s">
         <v>93</v>
       </c>
@@ -4795,8 +5082,11 @@
       <c r="K96">
         <v>365</v>
       </c>
-    </row>
-    <row r="97" spans="1:11">
+      <c r="O96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15">
       <c r="A97" t="s">
         <v>93</v>
       </c>
@@ -4830,8 +5120,11 @@
       <c r="K97">
         <v>365</v>
       </c>
-    </row>
-    <row r="98" spans="1:11">
+      <c r="O97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15">
       <c r="A98" t="s">
         <v>93</v>
       </c>
@@ -4865,8 +5158,11 @@
       <c r="K98">
         <v>365</v>
       </c>
-    </row>
-    <row r="99" spans="1:11">
+      <c r="O98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15">
       <c r="A99" t="s">
         <v>93</v>
       </c>
@@ -4900,8 +5196,11 @@
       <c r="K99">
         <v>365</v>
       </c>
-    </row>
-    <row r="100" spans="1:11">
+      <c r="O99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15">
       <c r="A100" t="s">
         <v>93</v>
       </c>
@@ -4935,8 +5234,11 @@
       <c r="K100">
         <v>365</v>
       </c>
-    </row>
-    <row r="101" spans="1:11">
+      <c r="O100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15">
       <c r="A101" t="s">
         <v>93</v>
       </c>
@@ -4970,8 +5272,11 @@
       <c r="K101">
         <v>365</v>
       </c>
-    </row>
-    <row r="102" spans="1:11">
+      <c r="O101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15">
       <c r="A102" t="s">
         <v>93</v>
       </c>
@@ -5005,8 +5310,11 @@
       <c r="K102">
         <v>365</v>
       </c>
-    </row>
-    <row r="103" spans="1:11">
+      <c r="O102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15">
       <c r="A103" t="s">
         <v>93</v>
       </c>
@@ -5040,8 +5348,11 @@
       <c r="K103">
         <v>365</v>
       </c>
-    </row>
-    <row r="104" spans="1:11">
+      <c r="O103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15">
       <c r="A104" t="s">
         <v>93</v>
       </c>
@@ -5075,8 +5386,11 @@
       <c r="K104">
         <v>365</v>
       </c>
-    </row>
-    <row r="105" spans="1:11">
+      <c r="O104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15">
       <c r="A105" t="s">
         <v>93</v>
       </c>
@@ -5110,8 +5424,11 @@
       <c r="K105">
         <v>365</v>
       </c>
-    </row>
-    <row r="106" spans="1:11">
+      <c r="O105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15">
       <c r="A106" t="s">
         <v>93</v>
       </c>
@@ -5145,8 +5462,11 @@
       <c r="K106">
         <v>365</v>
       </c>
-    </row>
-    <row r="107" spans="1:11">
+      <c r="O106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15">
       <c r="A107" t="s">
         <v>93</v>
       </c>
@@ -5180,8 +5500,11 @@
       <c r="K107">
         <v>365</v>
       </c>
-    </row>
-    <row r="108" spans="1:11">
+      <c r="O107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15">
       <c r="A108" t="s">
         <v>93</v>
       </c>
@@ -5215,8 +5538,11 @@
       <c r="K108">
         <v>365</v>
       </c>
-    </row>
-    <row r="109" spans="1:11">
+      <c r="O108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15">
       <c r="A109" t="s">
         <v>93</v>
       </c>
@@ -5250,8 +5576,11 @@
       <c r="K109">
         <v>365</v>
       </c>
-    </row>
-    <row r="110" spans="1:11">
+      <c r="O109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15">
       <c r="A110" t="s">
         <v>93</v>
       </c>
@@ -5285,8 +5614,11 @@
       <c r="K110">
         <v>365</v>
       </c>
-    </row>
-    <row r="111" spans="1:11">
+      <c r="O110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15">
       <c r="A111" t="s">
         <v>93</v>
       </c>
@@ -5320,8 +5652,11 @@
       <c r="K111">
         <v>365</v>
       </c>
-    </row>
-    <row r="112" spans="1:11">
+      <c r="O111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15">
       <c r="A112" t="s">
         <v>93</v>
       </c>
@@ -5355,8 +5690,11 @@
       <c r="K112">
         <v>365</v>
       </c>
-    </row>
-    <row r="113" spans="1:11">
+      <c r="O112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15">
       <c r="A113" t="s">
         <v>93</v>
       </c>
@@ -5390,8 +5728,11 @@
       <c r="K113">
         <v>365</v>
       </c>
-    </row>
-    <row r="114" spans="1:11">
+      <c r="O113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15">
       <c r="A114" t="s">
         <v>93</v>
       </c>
@@ -5425,8 +5766,11 @@
       <c r="K114">
         <v>365</v>
       </c>
-    </row>
-    <row r="115" spans="1:11">
+      <c r="O114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15">
       <c r="A115" t="s">
         <v>93</v>
       </c>
@@ -5460,8 +5804,11 @@
       <c r="K115">
         <v>365</v>
       </c>
-    </row>
-    <row r="116" spans="1:11">
+      <c r="O115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15">
       <c r="A116" t="s">
         <v>93</v>
       </c>
@@ -5495,8 +5842,11 @@
       <c r="K116">
         <v>365</v>
       </c>
-    </row>
-    <row r="117" spans="1:11">
+      <c r="O116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15">
       <c r="A117" t="s">
         <v>93</v>
       </c>
@@ -5530,8 +5880,11 @@
       <c r="K117">
         <v>365</v>
       </c>
-    </row>
-    <row r="118" spans="1:11">
+      <c r="O117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15">
       <c r="A118" t="s">
         <v>93</v>
       </c>
@@ -5565,8 +5918,11 @@
       <c r="K118">
         <v>365</v>
       </c>
-    </row>
-    <row r="119" spans="1:11">
+      <c r="O118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15">
       <c r="A119" t="s">
         <v>93</v>
       </c>
@@ -5600,8 +5956,11 @@
       <c r="K119">
         <v>365</v>
       </c>
-    </row>
-    <row r="120" spans="1:11">
+      <c r="O119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15">
       <c r="A120" t="s">
         <v>93</v>
       </c>
@@ -5635,8 +5994,11 @@
       <c r="K120">
         <v>365</v>
       </c>
-    </row>
-    <row r="121" spans="1:11">
+      <c r="O120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15">
       <c r="A121" t="s">
         <v>93</v>
       </c>
@@ -5670,8 +6032,11 @@
       <c r="K121">
         <v>365</v>
       </c>
-    </row>
-    <row r="122" spans="1:11">
+      <c r="O121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15">
       <c r="A122" t="s">
         <v>93</v>
       </c>
@@ -5705,8 +6070,11 @@
       <c r="K122">
         <v>365</v>
       </c>
-    </row>
-    <row r="123" spans="1:11">
+      <c r="O122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15">
       <c r="A123" t="s">
         <v>93</v>
       </c>
@@ -5740,8 +6108,11 @@
       <c r="K123">
         <v>365</v>
       </c>
-    </row>
-    <row r="124" spans="1:11">
+      <c r="O123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15">
       <c r="A124" t="s">
         <v>93</v>
       </c>
@@ -5775,8 +6146,11 @@
       <c r="K124">
         <v>365</v>
       </c>
-    </row>
-    <row r="125" spans="1:11">
+      <c r="O124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15">
       <c r="A125" t="s">
         <v>93</v>
       </c>
@@ -5810,8 +6184,11 @@
       <c r="K125">
         <v>365</v>
       </c>
-    </row>
-    <row r="126" spans="1:11">
+      <c r="O125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15">
       <c r="A126" t="s">
         <v>93</v>
       </c>
@@ -5845,8 +6222,11 @@
       <c r="K126">
         <v>365</v>
       </c>
-    </row>
-    <row r="127" spans="1:11">
+      <c r="O126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15">
       <c r="A127" t="s">
         <v>93</v>
       </c>
@@ -5880,8 +6260,11 @@
       <c r="K127">
         <v>365</v>
       </c>
-    </row>
-    <row r="128" spans="1:11">
+      <c r="O127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15">
       <c r="A128" t="s">
         <v>93</v>
       </c>
@@ -5915,8 +6298,11 @@
       <c r="K128">
         <v>365</v>
       </c>
-    </row>
-    <row r="129" spans="1:14">
+      <c r="O128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15">
       <c r="A129" t="s">
         <v>93</v>
       </c>
@@ -5950,8 +6336,11 @@
       <c r="K129">
         <v>365</v>
       </c>
-    </row>
-    <row r="130" spans="1:14">
+      <c r="O129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15">
       <c r="A130" t="s">
         <v>93</v>
       </c>
@@ -5985,8 +6374,11 @@
       <c r="K130">
         <v>365</v>
       </c>
-    </row>
-    <row r="131" spans="1:14">
+      <c r="O130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15">
       <c r="A131" t="s">
         <v>93</v>
       </c>
@@ -6020,8 +6412,11 @@
       <c r="N131">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:14">
+      <c r="O131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15">
       <c r="A132" t="s">
         <v>93</v>
       </c>
@@ -6055,8 +6450,11 @@
       <c r="K132">
         <v>30</v>
       </c>
-    </row>
-    <row r="133" spans="1:14">
+      <c r="O132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15">
       <c r="A133" t="s">
         <v>93</v>
       </c>
@@ -6090,8 +6488,11 @@
       <c r="K133">
         <v>30</v>
       </c>
-    </row>
-    <row r="134" spans="1:14">
+      <c r="O133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15">
       <c r="A134" t="s">
         <v>93</v>
       </c>
@@ -6122,8 +6523,11 @@
       <c r="J134">
         <v>5</v>
       </c>
-    </row>
-    <row r="135" spans="1:14">
+      <c r="O134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15">
       <c r="A135" t="s">
         <v>93</v>
       </c>
@@ -6154,8 +6558,11 @@
       <c r="J135">
         <v>5</v>
       </c>
-    </row>
-    <row r="136" spans="1:14">
+      <c r="O135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15">
       <c r="A136" t="s">
         <v>93</v>
       </c>
@@ -6186,8 +6593,11 @@
       <c r="J136">
         <v>5</v>
       </c>
-    </row>
-    <row r="137" spans="1:14">
+      <c r="O136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15">
       <c r="A137" t="s">
         <v>93</v>
       </c>
@@ -6218,8 +6628,11 @@
       <c r="J137">
         <v>5</v>
       </c>
-    </row>
-    <row r="138" spans="1:14">
+      <c r="O137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15">
       <c r="A138" t="s">
         <v>93</v>
       </c>
@@ -6250,8 +6663,11 @@
       <c r="K138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:14">
+      <c r="O138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15">
       <c r="A139" t="s">
         <v>93</v>
       </c>
@@ -6282,8 +6698,11 @@
       <c r="K139">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:14">
+      <c r="O139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15">
       <c r="A140" t="s">
         <v>93</v>
       </c>
@@ -6317,8 +6736,11 @@
       <c r="N140">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:14">
+      <c r="O140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15">
       <c r="A141" t="s">
         <v>93</v>
       </c>
@@ -6352,8 +6774,11 @@
       <c r="K141">
         <v>30</v>
       </c>
-    </row>
-    <row r="142" spans="1:14">
+      <c r="O141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15">
       <c r="A142" t="s">
         <v>93</v>
       </c>
@@ -6387,8 +6812,11 @@
       <c r="K142">
         <v>30</v>
       </c>
-    </row>
-    <row r="143" spans="1:14">
+      <c r="O142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15">
       <c r="A143" t="s">
         <v>93</v>
       </c>
@@ -6422,8 +6850,11 @@
       <c r="K143">
         <v>30</v>
       </c>
-    </row>
-    <row r="144" spans="1:14">
+      <c r="O143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15">
       <c r="A144" t="s">
         <v>93</v>
       </c>
@@ -6457,8 +6888,11 @@
       <c r="K144">
         <v>30</v>
       </c>
-    </row>
-    <row r="145" spans="1:14">
+      <c r="O144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15">
       <c r="A145" t="s">
         <v>93</v>
       </c>
@@ -6492,8 +6926,11 @@
       <c r="K145">
         <v>30</v>
       </c>
-    </row>
-    <row r="146" spans="1:14">
+      <c r="O145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15">
       <c r="A146" t="s">
         <v>93</v>
       </c>
@@ -6527,8 +6964,11 @@
       <c r="K146">
         <v>30</v>
       </c>
-    </row>
-    <row r="147" spans="1:14">
+      <c r="O146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15">
       <c r="A147" t="s">
         <v>93</v>
       </c>
@@ -6559,8 +6999,11 @@
       <c r="K147">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:14">
+      <c r="O147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15">
       <c r="A148" t="s">
         <v>93</v>
       </c>
@@ -6591,8 +7034,11 @@
       <c r="K148">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:14">
+      <c r="O148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15">
       <c r="A149" t="s">
         <v>93</v>
       </c>
@@ -6623,8 +7069,11 @@
       <c r="K149">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:14">
+      <c r="O149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15">
       <c r="A150" t="s">
         <v>93</v>
       </c>
@@ -6655,8 +7104,11 @@
       <c r="K150">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="1:14">
+      <c r="O150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15">
       <c r="A151" t="s">
         <v>93</v>
       </c>
@@ -6687,8 +7139,11 @@
       <c r="K151">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:14">
+      <c r="O151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15">
       <c r="A152" t="s">
         <v>93</v>
       </c>
@@ -6722,8 +7177,11 @@
       <c r="K152">
         <v>30</v>
       </c>
-    </row>
-    <row r="153" spans="1:14">
+      <c r="O152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15">
       <c r="A153" t="s">
         <v>93</v>
       </c>
@@ -6757,8 +7215,11 @@
       <c r="K153">
         <v>30</v>
       </c>
-    </row>
-    <row r="154" spans="1:14">
+      <c r="O153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15">
       <c r="A154" t="s">
         <v>93</v>
       </c>
@@ -6792,8 +7253,11 @@
       <c r="K154">
         <v>30</v>
       </c>
-    </row>
-    <row r="155" spans="1:14">
+      <c r="O154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15">
       <c r="A155" t="s">
         <v>93</v>
       </c>
@@ -6827,8 +7291,11 @@
       <c r="K155">
         <v>30</v>
       </c>
-    </row>
-    <row r="156" spans="1:14">
+      <c r="O155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15">
       <c r="A156" t="s">
         <v>93</v>
       </c>
@@ -6862,8 +7329,11 @@
       <c r="K156">
         <v>30</v>
       </c>
-    </row>
-    <row r="157" spans="1:14">
+      <c r="O156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15">
       <c r="A157" t="s">
         <v>93</v>
       </c>
@@ -6897,8 +7367,11 @@
       <c r="N157">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:14">
+      <c r="O157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15">
       <c r="A158" t="s">
         <v>93</v>
       </c>
@@ -6932,8 +7405,11 @@
       <c r="N158">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:14">
+      <c r="O158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15">
       <c r="A159" t="s">
         <v>93</v>
       </c>
@@ -6967,8 +7443,11 @@
       <c r="N159">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:14">
+      <c r="O159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15">
       <c r="A160" t="s">
         <v>93</v>
       </c>
@@ -7002,8 +7481,11 @@
       <c r="N160">
         <v>1</v>
       </c>
-    </row>
-    <row r="161" spans="1:14">
+      <c r="O160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15">
       <c r="A161" t="s">
         <v>93</v>
       </c>
@@ -7037,8 +7519,11 @@
       <c r="N161">
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="1:14">
+      <c r="O161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15">
       <c r="A162" t="s">
         <v>93</v>
       </c>
@@ -7069,8 +7554,11 @@
       <c r="N162">
         <v>1</v>
       </c>
-    </row>
-    <row r="163" spans="1:14">
+      <c r="O162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15">
       <c r="A163" t="s">
         <v>93</v>
       </c>
@@ -7101,14 +7589,14 @@
       <c r="J163">
         <v>2</v>
       </c>
-      <c r="K163">
-        <v>30</v>
-      </c>
       <c r="N163">
         <v>1</v>
       </c>
-    </row>
-    <row r="164" spans="1:14">
+      <c r="O163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15">
       <c r="A164" t="s">
         <v>93</v>
       </c>
@@ -7139,14 +7627,14 @@
       <c r="J164">
         <v>2</v>
       </c>
-      <c r="K164">
-        <v>30</v>
-      </c>
       <c r="N164">
         <v>1</v>
       </c>
-    </row>
-    <row r="165" spans="1:14">
+      <c r="O164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15">
       <c r="A165" t="s">
         <v>93</v>
       </c>
@@ -7180,8 +7668,11 @@
       <c r="N165">
         <v>1</v>
       </c>
-    </row>
-    <row r="166" spans="1:14">
+      <c r="O165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15">
       <c r="A166" t="s">
         <v>93</v>
       </c>
@@ -7203,7 +7694,7 @@
       <c r="G166" t="s">
         <v>3</v>
       </c>
-      <c r="H166" s="7" t="s">
+      <c r="H166" t="s">
         <v>37</v>
       </c>
       <c r="I166" t="s">
@@ -7215,8 +7706,11 @@
       <c r="N166">
         <v>1</v>
       </c>
-    </row>
-    <row r="167" spans="1:14">
+      <c r="O166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15">
       <c r="A167" t="s">
         <v>93</v>
       </c>
@@ -7238,7 +7732,7 @@
       <c r="G167" t="s">
         <v>3</v>
       </c>
-      <c r="H167" s="7" t="s">
+      <c r="H167" t="s">
         <v>37</v>
       </c>
       <c r="I167" t="s">
@@ -7250,8 +7744,11 @@
       <c r="K167">
         <v>365</v>
       </c>
-    </row>
-    <row r="168" spans="1:14">
+      <c r="O167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15">
       <c r="A168" t="s">
         <v>93</v>
       </c>
@@ -7273,7 +7770,7 @@
       <c r="G168" t="s">
         <v>3</v>
       </c>
-      <c r="H168" s="7" t="s">
+      <c r="H168" t="s">
         <v>37</v>
       </c>
       <c r="I168" t="s">
@@ -7285,8 +7782,11 @@
       <c r="K168">
         <v>365</v>
       </c>
-    </row>
-    <row r="169" spans="1:14">
+      <c r="O168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15">
       <c r="A169" t="s">
         <v>93</v>
       </c>
@@ -7308,7 +7808,7 @@
       <c r="G169" t="s">
         <v>3</v>
       </c>
-      <c r="H169" s="7" t="s">
+      <c r="H169" t="s">
         <v>37</v>
       </c>
       <c r="I169" t="s">
@@ -7320,8 +7820,11 @@
       <c r="K169">
         <v>365</v>
       </c>
-    </row>
-    <row r="170" spans="1:14">
+      <c r="O169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15">
       <c r="A170" t="s">
         <v>93</v>
       </c>
@@ -7343,7 +7846,7 @@
       <c r="G170" t="s">
         <v>3</v>
       </c>
-      <c r="H170" s="7" t="s">
+      <c r="H170" t="s">
         <v>37</v>
       </c>
       <c r="I170" t="s">
@@ -7355,8 +7858,11 @@
       <c r="K170">
         <v>365</v>
       </c>
-    </row>
-    <row r="171" spans="1:14">
+      <c r="O170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15">
       <c r="A171" t="s">
         <v>93</v>
       </c>
@@ -7378,7 +7884,7 @@
       <c r="G171" t="s">
         <v>3</v>
       </c>
-      <c r="H171" s="7" t="s">
+      <c r="H171" t="s">
         <v>37</v>
       </c>
       <c r="I171" t="s">
@@ -7387,8 +7893,11 @@
       <c r="K171">
         <v>365</v>
       </c>
-    </row>
-    <row r="172" spans="1:14">
+      <c r="O171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15">
       <c r="A172" t="s">
         <v>93</v>
       </c>
@@ -7410,7 +7919,7 @@
       <c r="G172" t="s">
         <v>3</v>
       </c>
-      <c r="H172" s="7" t="s">
+      <c r="H172" t="s">
         <v>37</v>
       </c>
       <c r="I172" t="s">
@@ -7419,8 +7928,11 @@
       <c r="K172">
         <v>365</v>
       </c>
-    </row>
-    <row r="173" spans="1:14">
+      <c r="O172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15">
       <c r="A173" t="s">
         <v>93</v>
       </c>
@@ -7442,7 +7954,7 @@
       <c r="G173" t="s">
         <v>3</v>
       </c>
-      <c r="H173" s="7" t="s">
+      <c r="H173" t="s">
         <v>37</v>
       </c>
       <c r="I173" t="s">
@@ -7451,8 +7963,11 @@
       <c r="K173">
         <v>365</v>
       </c>
-    </row>
-    <row r="174" spans="1:14">
+      <c r="O173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15">
       <c r="A174" t="s">
         <v>93</v>
       </c>
@@ -7474,7 +7989,7 @@
       <c r="G174" t="s">
         <v>3</v>
       </c>
-      <c r="H174" s="7" t="s">
+      <c r="H174" t="s">
         <v>37</v>
       </c>
       <c r="I174" t="s">
@@ -7486,8 +8001,11 @@
       <c r="K174">
         <v>365</v>
       </c>
-    </row>
-    <row r="175" spans="1:14">
+      <c r="O174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15">
       <c r="A175" t="s">
         <v>93</v>
       </c>
@@ -7509,7 +8027,7 @@
       <c r="G175" t="s">
         <v>3</v>
       </c>
-      <c r="H175" s="7" t="s">
+      <c r="H175" t="s">
         <v>37</v>
       </c>
       <c r="I175" t="s">
@@ -7521,8 +8039,11 @@
       <c r="K175">
         <v>365</v>
       </c>
-    </row>
-    <row r="176" spans="1:14">
+      <c r="O175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15">
       <c r="A176" t="s">
         <v>93</v>
       </c>
@@ -7544,7 +8065,7 @@
       <c r="G176" t="s">
         <v>3</v>
       </c>
-      <c r="H176" s="7" t="s">
+      <c r="H176" t="s">
         <v>37</v>
       </c>
       <c r="I176" t="s">
@@ -7556,8 +8077,11 @@
       <c r="K176">
         <v>365</v>
       </c>
-    </row>
-    <row r="177" spans="1:11">
+      <c r="O176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15">
       <c r="A177" t="s">
         <v>93</v>
       </c>
@@ -7579,7 +8103,7 @@
       <c r="G177" t="s">
         <v>3</v>
       </c>
-      <c r="H177" s="7" t="s">
+      <c r="H177" t="s">
         <v>37</v>
       </c>
       <c r="I177" t="s">
@@ -7591,8 +8115,11 @@
       <c r="K177">
         <v>365</v>
       </c>
-    </row>
-    <row r="178" spans="1:11">
+      <c r="O177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15">
       <c r="A178" t="s">
         <v>93</v>
       </c>
@@ -7614,7 +8141,7 @@
       <c r="G178" t="s">
         <v>3</v>
       </c>
-      <c r="H178" s="7" t="s">
+      <c r="H178" t="s">
         <v>37</v>
       </c>
       <c r="I178" t="s">
@@ -7626,8 +8153,11 @@
       <c r="K178">
         <v>365</v>
       </c>
-    </row>
-    <row r="179" spans="1:11">
+      <c r="O178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15">
       <c r="A179" t="s">
         <v>93</v>
       </c>
@@ -7649,7 +8179,7 @@
       <c r="G179" t="s">
         <v>3</v>
       </c>
-      <c r="H179" s="7" t="s">
+      <c r="H179" t="s">
         <v>37</v>
       </c>
       <c r="I179" t="s">
@@ -7661,8 +8191,11 @@
       <c r="K179">
         <v>365</v>
       </c>
-    </row>
-    <row r="180" spans="1:11">
+      <c r="O179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15">
       <c r="A180" t="s">
         <v>93</v>
       </c>
@@ -7684,7 +8217,7 @@
       <c r="G180" t="s">
         <v>3</v>
       </c>
-      <c r="H180" s="7" t="s">
+      <c r="H180" t="s">
         <v>37</v>
       </c>
       <c r="I180" t="s">
@@ -7696,8 +8229,11 @@
       <c r="K180">
         <v>365</v>
       </c>
-    </row>
-    <row r="181" spans="1:11">
+      <c r="O180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15">
       <c r="A181" t="s">
         <v>93</v>
       </c>
@@ -7719,7 +8255,7 @@
       <c r="G181" t="s">
         <v>3</v>
       </c>
-      <c r="H181" s="7" t="s">
+      <c r="H181" t="s">
         <v>37</v>
       </c>
       <c r="I181" t="s">
@@ -7731,8 +8267,11 @@
       <c r="K181">
         <v>365</v>
       </c>
-    </row>
-    <row r="182" spans="1:11">
+      <c r="O181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15">
       <c r="A182" t="s">
         <v>93</v>
       </c>
@@ -7754,7 +8293,7 @@
       <c r="G182" t="s">
         <v>3</v>
       </c>
-      <c r="H182" s="7" t="s">
+      <c r="H182" t="s">
         <v>37</v>
       </c>
       <c r="I182" t="s">
@@ -7766,8 +8305,11 @@
       <c r="K182">
         <v>365</v>
       </c>
-    </row>
-    <row r="183" spans="1:11">
+      <c r="O182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15">
       <c r="A183" t="s">
         <v>93</v>
       </c>
@@ -7789,7 +8331,7 @@
       <c r="G183" t="s">
         <v>3</v>
       </c>
-      <c r="H183" s="7" t="s">
+      <c r="H183" t="s">
         <v>37</v>
       </c>
       <c r="I183" t="s">
@@ -7801,8 +8343,11 @@
       <c r="K183">
         <v>365</v>
       </c>
-    </row>
-    <row r="184" spans="1:11">
+      <c r="O183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15">
       <c r="A184" t="s">
         <v>93</v>
       </c>
@@ -7824,7 +8369,7 @@
       <c r="G184" t="s">
         <v>3</v>
       </c>
-      <c r="H184" s="7" t="s">
+      <c r="H184" t="s">
         <v>37</v>
       </c>
       <c r="I184" t="s">
@@ -7836,8 +8381,11 @@
       <c r="K184">
         <v>365</v>
       </c>
-    </row>
-    <row r="185" spans="1:11">
+      <c r="O184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15">
       <c r="A185" t="s">
         <v>93</v>
       </c>
@@ -7859,7 +8407,7 @@
       <c r="G185" t="s">
         <v>3</v>
       </c>
-      <c r="H185" s="7" t="s">
+      <c r="H185" t="s">
         <v>37</v>
       </c>
       <c r="I185" t="s">
@@ -7870,6 +8418,9 @@
       </c>
       <c r="K185">
         <v>365</v>
+      </c>
+      <c r="O185">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7880,10 +8431,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O136"/>
+  <dimension ref="A1:P136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7892,7 +8443,7 @@
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>148</v>
       </c>
@@ -7936,10 +8487,13 @@
         <v>155</v>
       </c>
       <c r="O1" t="s">
+        <v>343</v>
+      </c>
+      <c r="P1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17" customHeight="1">
+    <row r="2" spans="1:16" ht="17" customHeight="1">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -7955,11 +8509,11 @@
       <c r="E2" t="s">
         <v>95</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17" customHeight="1">
+    <row r="3" spans="1:16" ht="17" customHeight="1">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -7975,11 +8529,11 @@
       <c r="E3" t="s">
         <v>95</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="17" customHeight="1">
+    <row r="4" spans="1:16" ht="17" customHeight="1">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -7995,11 +8549,11 @@
       <c r="E4" t="s">
         <v>95</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="17" customHeight="1">
+    <row r="5" spans="1:16" ht="17" customHeight="1">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -8015,11 +8569,11 @@
       <c r="E5" t="s">
         <v>95</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="17">
+    <row r="6" spans="1:16" ht="17">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -8035,75 +8589,76 @@
       <c r="E6" t="s">
         <v>95</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:16">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="4:15">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4">
+    <row r="18" spans="4:15">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="4:4">
+    <row r="19" spans="4:15">
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="4:4">
+    <row r="20" spans="4:15">
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="4:4">
+    <row r="21" spans="4:15">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="4:4">
+    <row r="22" spans="4:15">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="4:4">
+    <row r="23" spans="4:15">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="4:4">
+    <row r="24" spans="4:15">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="4:4">
+    <row r="25" spans="4:15">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:4">
+    <row r="26" spans="4:15">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="4:4">
+    <row r="27" spans="4:15">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="4:4">
+    <row r="28" spans="4:15" ht="19">
       <c r="D28" s="4"/>
+      <c r="O28" s="3"/>
     </row>
     <row r="56" spans="4:4">
       <c r="D56" s="4"/>
@@ -8275,10 +8830,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8286,7 +8841,7 @@
     <col min="3" max="3" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>148</v>
       </c>
@@ -8330,10 +8885,13 @@
         <v>155</v>
       </c>
       <c r="O1" t="s">
+        <v>343</v>
+      </c>
+      <c r="P1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -8349,11 +8907,11 @@
       <c r="E2" t="s">
         <v>119</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -8369,11 +8927,11 @@
       <c r="E3" t="s">
         <v>119</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -8389,11 +8947,11 @@
       <c r="E4" t="s">
         <v>119</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -8409,11 +8967,11 @@
       <c r="E5" t="s">
         <v>119</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -8429,11 +8987,11 @@
       <c r="E6" t="s">
         <v>120</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -8449,11 +9007,11 @@
       <c r="E7" t="s">
         <v>120</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -8469,11 +9027,11 @@
       <c r="E8" t="s">
         <v>120</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -8489,11 +9047,11 @@
       <c r="E9" t="s">
         <v>120</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>93</v>
       </c>
@@ -8509,11 +9067,11 @@
       <c r="E10" t="s">
         <v>121</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>93</v>
       </c>
@@ -8529,11 +9087,11 @@
       <c r="E11" t="s">
         <v>121</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>93</v>
       </c>
@@ -8549,11 +9107,11 @@
       <c r="E12" t="s">
         <v>120</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -8569,9 +9127,12 @@
       <c r="E13" t="s">
         <v>119</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>281</v>
       </c>
+    </row>
+    <row r="28" spans="15:15" ht="19">
+      <c r="O28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8581,10 +9142,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8593,7 +9154,7 @@
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>148</v>
       </c>
@@ -8637,10 +9198,13 @@
         <v>155</v>
       </c>
       <c r="O1" t="s">
+        <v>343</v>
+      </c>
+      <c r="P1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -8656,11 +9220,11 @@
       <c r="E2" t="s">
         <v>99</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -8676,11 +9240,11 @@
       <c r="E3" t="s">
         <v>99</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -8696,11 +9260,11 @@
       <c r="E4" t="s">
         <v>99</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -8716,11 +9280,11 @@
       <c r="E5" t="s">
         <v>99</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -8736,11 +9300,11 @@
       <c r="E6" t="s">
         <v>100</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -8756,11 +9320,11 @@
       <c r="E7" t="s">
         <v>100</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -8776,11 +9340,11 @@
       <c r="E8" t="s">
         <v>100</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -8796,11 +9360,11 @@
       <c r="E9" t="s">
         <v>100</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>93</v>
       </c>
@@ -8816,11 +9380,11 @@
       <c r="E10" t="s">
         <v>101</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>93</v>
       </c>
@@ -8836,11 +9400,11 @@
       <c r="E11" t="s">
         <v>101</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>93</v>
       </c>
@@ -8856,11 +9420,11 @@
       <c r="E12" t="s">
         <v>101</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -8876,11 +9440,11 @@
       <c r="E13" t="s">
         <v>101</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -8896,11 +9460,11 @@
       <c r="E14" t="s">
         <v>99</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -8916,12 +9480,13 @@
       <c r="E15" t="s">
         <v>101</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="28" spans="6:6" ht="17" customHeight="1">
+    <row r="28" spans="6:15" ht="17" customHeight="1">
       <c r="F28" s="5"/>
+      <c r="O28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8931,10 +9496,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8942,7 +9507,7 @@
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>148</v>
       </c>
@@ -8986,14 +9551,20 @@
         <v>155</v>
       </c>
       <c r="O1" t="s">
+        <v>343</v>
+      </c>
+      <c r="P1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="P6" s="6"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="P7" s="6"/>
+    <row r="6" spans="1:17">
+      <c r="Q6" s="6"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="Q7" s="6"/>
+    </row>
+    <row r="28" spans="15:15" ht="19">
+      <c r="O28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9005,7 +9576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1C4AD9-240E-DF4B-A8B9-797210EF8A3C}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>

</xml_diff>